<commit_message>
Deploy cccdc13 from branch develop
</commit_message>
<xml_diff>
--- a/public/AddInfos/de/7.1.2.xlsx
+++ b/public/AddInfos/de/7.1.2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>Jahr</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>Bevölkerung mit überwiegender Abhängigkeit von sauberen Energieträgern und Technologien</t>
+  </si>
+  <si>
+    <t>Datenquelle:</t>
+  </si>
+  <si>
+    <t>Weltgesundheitsorganisation (WHO)</t>
   </si>
 </sst>
 </file>
@@ -431,18 +437,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -454,9 +461,8 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -468,9 +474,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2010</v>
       </c>
@@ -482,9 +487,8 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2011</v>
       </c>
@@ -496,9 +500,8 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2012</v>
       </c>
@@ -510,9 +513,8 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2013</v>
       </c>
@@ -524,9 +526,8 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2014</v>
       </c>
@@ -538,9 +539,8 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>2015</v>
       </c>
@@ -552,9 +552,8 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>2016</v>
       </c>
@@ -566,9 +565,8 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -576,7 +574,109 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Deploy 4ac4bbf from branch develop
</commit_message>
<xml_diff>
--- a/public/AddInfos/de/7.1.2.xlsx
+++ b/public/AddInfos/de/7.1.2.xlsx
@@ -142,12 +142,370 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFCC30B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1600"/>
+              <a:t>Bevölkerung mit überwiegender Abhängigkeit von sauberen Energieträgern und Technologien</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:noFill/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle2!$A$1:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle2!$B$1:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FCC30B"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle2!$A$1:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle2!$C$1:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="59719168"/>
+        <c:axId val="78547200"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="59719168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Jahr</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78547200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="78547200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Prozent (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="59719168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571324</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>571429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1409524" cy="571429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -437,63 +795,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-    </row>
-    <row r="2" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
+    <row r="1" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2010</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>2011</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>2</v>
+    <row r="3" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -503,7 +855,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>2</v>
@@ -516,7 +868,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>2</v>
@@ -529,7 +881,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>2</v>
@@ -542,7 +894,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>2</v>
@@ -555,7 +907,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>2</v>
@@ -567,8 +919,12 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="4">
+        <v>2015</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -576,11 +932,11 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
+      <c r="A11" s="4">
+        <v>2016</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -678,23 +1034,270 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4">
+        <v>2010</v>
+      </c>
+      <c r="B1">
+        <v>95</v>
+      </c>
+      <c r="C1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>2011</v>
+      </c>
+      <c r="B2">
+        <v>95</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2012</v>
+      </c>
+      <c r="B3">
+        <v>95</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2013</v>
+      </c>
+      <c r="B4">
+        <v>95</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2014</v>
+      </c>
+      <c r="B5">
+        <v>95</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>2015</v>
+      </c>
+      <c r="B6">
+        <v>95</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>2016</v>
+      </c>
+      <c r="B7">
+        <v>95</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Deploy 5510f07 from branch develop
</commit_message>
<xml_diff>
--- a/public/AddInfos/de/7.1.2.xlsx
+++ b/public/AddInfos/de/7.1.2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Jahr</t>
   </si>
@@ -38,12 +38,21 @@
   <si>
     <t>Weltgesundheitsorganisation (WHO)</t>
   </si>
+  <si>
+    <t xml:space="preserve">Copyright: </t>
+  </si>
+  <si>
+    <t>©       Statistisches Bundesamt (Destatis) 2020</t>
+  </si>
+  <si>
+    <t>Vervielfältigung und Verbreitung, auch auszugsweise, mit Quellenangaben gestattet.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +67,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -115,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -136,6 +158,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -338,11 +362,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="59719168"/>
-        <c:axId val="78547200"/>
+        <c:axId val="82498560"/>
+        <c:axId val="41267136"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="59719168"/>
+        <c:axId val="82498560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -372,7 +396,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78547200"/>
+        <c:crossAx val="41267136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -380,7 +404,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78547200"/>
+        <c:axId val="41267136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -412,7 +436,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59719168"/>
+        <c:crossAx val="82498560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -466,23 +490,23 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1245</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>571324</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>571429</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>365045</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Grafik 2"/>
+        <xdr:cNvPr id="5" name="Grafik 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -495,8 +519,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1409524" cy="571429"/>
+          <a:off x="0" y="1245"/>
+          <a:ext cx="1973179" cy="715637"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>149088</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>41412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>291945</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>184269</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Grafik 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1018762" y="7810499"/>
+          <a:ext cx="142857" cy="142857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -795,15 +863,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="6.85546875" customWidth="1"/>
     <col min="8" max="8" width="5.28515625" style="1" customWidth="1"/>
@@ -1152,31 +1220,37 @@
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="1"/>
+      <c r="C35" s="8"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="A36" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="8"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="8"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -1199,6 +1273,24 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Deploy 4ffca36 from branch develop
</commit_message>
<xml_diff>
--- a/public/AddInfos/de/7.1.2.xlsx
+++ b/public/AddInfos/de/7.1.2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>Jahr</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Datenquelle:</t>
   </si>
   <si>
-    <t>Weltgesundheitsorganisation (WHO)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Copyright: </t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>Vervielfältigung und Verbreitung, auch auszugsweise, mit Quellenangaben gestattet.</t>
+  </si>
+  <si>
+    <t>Weltgesundheitsorganisation (WHO), Stand 11.04.2019</t>
   </si>
 </sst>
 </file>
@@ -155,11 +155,11 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -226,10 +226,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle2!$A$1:$A$7</c:f>
+              <c:f>Tabelle2!$A$1:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -250,16 +250,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$B$1:$B$7</c:f>
+              <c:f>Tabelle2!$B$1:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>95</c:v>
                 </c:pt>
@@ -279,6 +282,9 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>95</c:v>
                 </c:pt>
               </c:numCache>
@@ -295,10 +301,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle2!$A$1:$A$7</c:f>
+              <c:f>Tabelle2!$A$1:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>2010</c:v>
                 </c:pt>
@@ -319,16 +325,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$C$1:$C$7</c:f>
+              <c:f>Tabelle2!$C$1:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -348,6 +357,9 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -362,11 +374,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="82498560"/>
-        <c:axId val="41267136"/>
+        <c:axId val="178840576"/>
+        <c:axId val="41266560"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="82498560"/>
+        <c:axId val="178840576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -396,7 +408,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41267136"/>
+        <c:crossAx val="41266560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -404,7 +416,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41267136"/>
+        <c:axId val="41266560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -436,7 +448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82498560"/>
+        <c:crossAx val="178840576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -865,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,14 +911,14 @@
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -1013,8 +1025,12 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1220,37 +1236,37 @@
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="8"/>
+      <c r="B35" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="7"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="8"/>
+      <c r="C36" s="7"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="8"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="7"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -1304,10 +1320,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,6 +1402,17 @@
         <v>95</v>
       </c>
       <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B8">
+        <v>95</v>
+      </c>
+      <c r="C8">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 7e56edd16ac69c822dd69889c3e0011bb70a9c61 🚀
</commit_message>
<xml_diff>
--- a/public/AddInfos/de/7.1.2.xlsx
+++ b/public/AddInfos/de/7.1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dauerausleihe04\Documents\SDG\SdgTestEnvironment\sdg-indicators\public\AddInfos\de\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626E6089-B4AE-4DA2-A867-808310B59A32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD1F4DE-1618-49EC-8A6B-D1F60E4AD9AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="96" windowWidth="28512" windowHeight="13296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,21 +22,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Jahr</t>
-  </si>
-  <si>
-    <t>Wert in Prozent</t>
   </si>
   <si>
     <t>&gt; 95</t>
   </si>
   <si>
     <t>7.1.2</t>
-  </si>
-  <si>
-    <t>Bevölkerung mit überwiegender Abhängigkeit von sauberen Energieträgern und Technologien</t>
   </si>
   <si>
     <t>Datenquelle:</t>
@@ -52,6 +46,18 @@
   </si>
   <si>
     <t>©       Statistisches Bundesamt (Destatis) 2021</t>
+  </si>
+  <si>
+    <t>Anteil der Bevölkerung, der vorwiegend saubere Energieträger und Technologien nutzt</t>
+  </si>
+  <si>
+    <t>Prozent</t>
+  </si>
+  <si>
+    <t>Anmerkung:</t>
+  </si>
+  <si>
+    <t>Alle Daten geschätzt.</t>
   </si>
 </sst>
 </file>
@@ -591,13 +597,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>149088</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>41412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>291945</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>1389</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -961,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -995,10 +1001,10 @@
     </row>
     <row r="3" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -1006,12 +1012,12 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1024,7 +1030,7 @@
         <v>2010</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1037,7 +1043,7 @@
         <v>2011</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1050,7 +1056,7 @@
         <v>2012</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1063,7 +1069,7 @@
         <v>2013</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1076,7 +1082,7 @@
         <v>2014</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1089,7 +1095,7 @@
         <v>2015</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1102,7 +1108,7 @@
         <v>2016</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1115,7 +1121,7 @@
         <v>2017</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1128,7 +1134,7 @@
         <v>2018</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1141,7 +1147,7 @@
         <v>2019</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1154,7 +1160,7 @@
         <v>2020</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1344,10 +1350,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="1"/>
@@ -1357,10 +1363,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="1"/>
@@ -1369,8 +1375,10 @@
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7" t="s">
+      <c r="A38" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C38" s="7"/>
@@ -1380,9 +1388,11 @@
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="7"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -1396,6 +1406,15 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>